<commit_message>
último commit en el ces
</commit_message>
<xml_diff>
--- a/plan_trabajo.xlsx
+++ b/plan_trabajo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlpome\OneDrive - Seguros Suramericana, S.A\Escritorio\dataton_make_health\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25ABB9D7-C325-43BC-98F5-60449AEFDEFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887E414E-4AE4-4006-AFA3-AC8F73FF721F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5181BF0A-CBCB-49E2-861F-A0497D548C7C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>investigación en determinantes del dengue</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Clara</t>
   </si>
   <si>
-    <t>Joha, David, Daniel</t>
-  </si>
-  <si>
     <t>Joha?</t>
   </si>
   <si>
@@ -103,6 +100,24 @@
   </si>
   <si>
     <t>cluster de los municipios - características</t>
+  </si>
+  <si>
+    <t>*tendencias de tasa de los municipios con tasa más alta</t>
+  </si>
+  <si>
+    <t>agregar las variables a los features ya creados</t>
+  </si>
+  <si>
+    <t>felipe</t>
+  </si>
+  <si>
+    <t>esteban</t>
+  </si>
+  <si>
+    <t>modelo predicción casos mensuales</t>
+  </si>
+  <si>
+    <t>David, Daniel</t>
   </si>
 </sst>
 </file>
@@ -454,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30BDBD0C-6618-47C2-A0B6-BC3F276953B5}">
-  <dimension ref="D3:E34"/>
+  <dimension ref="D3:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,30 +503,50 @@
     </row>
     <row r="11" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>5</v>
       </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>6</v>
       </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>7</v>
       </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
@@ -544,6 +579,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>2</v>
@@ -559,20 +602,34 @@
     </row>
     <row r="31" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>